<commit_message>
see readme for updates
</commit_message>
<xml_diff>
--- a/datalinkage/output/bob_out.xlsx
+++ b/datalinkage/output/bob_out.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16027" uniqueCount="57">
   <si>
-    <t>date_sign_up</t>
+    <t>date</t>
   </si>
   <si>
     <t>customer_id</t>
   </si>
   <si>
-    <t>Employee ID</t>
+    <t>eid</t>
   </si>
   <si>
-    <t>Office</t>
+    <t>office</t>
   </si>
   <si>
-    <t>Box Type</t>
+    <t>box_type</t>
   </si>
   <si>
     <t>03/11/19</t>

</xml_diff>